<commit_message>
RDM-12853 Add CallbackGetCaseUrl and retries to the CaseType
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_CNP_RDM5118.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_CNP_RDM5118.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleynoronha/code/ccd/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D882BBF2-E20A-0A4F-8AB6-FA2A3CE0051D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1FA6DF-7CB2-6E47-98A1-9B9005B9D734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="29180" windowHeight="16620" tabRatio="823" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="56960" yWindow="6040" windowWidth="29180" windowHeight="16620" tabRatio="823" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7349" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7354" uniqueCount="308">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -971,6 +971,23 @@
   <si>
     <t>CUSTOM  TITLE DISPLAY</t>
   </si>
+  <si>
+    <t>URL to call back to the service for uniqueness. 
+Max Length: &lt;unlimited&gt;</t>
+  </si>
+  <si>
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
+MaxLength: &lt;unlimited&gt;</t>
+  </si>
+  <si>
+    <t>CallbackGetCaseUrl</t>
+  </si>
+  <si>
+    <t>RetriesGetCaseUrl</t>
+  </si>
+  <si>
+    <t>${TEST_STUB_SERVICE_BASE_URL:http://ccd-test-stubs-service-aat.service.core-compute-aat.internal}/case_type/fe-functional-test/callback_get_case</t>
+  </si>
 </sst>
 </file>
 
@@ -981,7 +998,7 @@
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1260,8 +1277,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1290,6 +1313,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0432FF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1378,7 +1407,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1501,6 +1530,12 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -15635,10 +15670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15652,9 +15687,11 @@
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="11" max="11" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -15673,7 +15710,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" s="30" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" s="30" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -15697,8 +15734,14 @@
       <c r="I2" s="31" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J2" s="88" t="s">
+        <v>303</v>
+      </c>
+      <c r="K2" s="88" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -15726,8 +15769,14 @@
       <c r="I3" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J3" s="89" t="s">
+        <v>305</v>
+      </c>
+      <c r="K3" s="89" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -15747,8 +15796,11 @@
       <c r="I4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -15769,7 +15821,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -15792,7 +15844,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -15815,7 +15867,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -15838,7 +15890,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -15861,7 +15913,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -15884,7 +15936,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -20496,7 +20548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding other def files
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_CNP_RDM5118.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_CNP_RDM5118.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ashleynoronha/code/ccd/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D882BBF2-E20A-0A4F-8AB6-FA2A3CE0051D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1FA6DF-7CB2-6E47-98A1-9B9005B9D734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1080" windowWidth="29180" windowHeight="16620" tabRatio="823" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="56960" yWindow="6040" windowWidth="29180" windowHeight="16620" tabRatio="823" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7349" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7354" uniqueCount="308">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -971,6 +971,23 @@
   <si>
     <t>CUSTOM  TITLE DISPLAY</t>
   </si>
+  <si>
+    <t>URL to call back to the service for uniqueness. 
+Max Length: &lt;unlimited&gt;</t>
+  </si>
+  <si>
+    <t>Comma separate timeout (each number is a retry , seconds e.g. 5,10,15 = three retries with increasing timeout time). 
+MaxLength: &lt;unlimited&gt;</t>
+  </si>
+  <si>
+    <t>CallbackGetCaseUrl</t>
+  </si>
+  <si>
+    <t>RetriesGetCaseUrl</t>
+  </si>
+  <si>
+    <t>${TEST_STUB_SERVICE_BASE_URL:http://ccd-test-stubs-service-aat.service.core-compute-aat.internal}/case_type/fe-functional-test/callback_get_case</t>
+  </si>
 </sst>
 </file>
 
@@ -981,7 +998,7 @@
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="42" x14ac:knownFonts="1">
+  <fonts count="43" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1260,8 +1277,14 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1290,6 +1313,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0432FF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1378,7 +1407,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1501,6 +1530,12 @@
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="26" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="42" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="29">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -15635,10 +15670,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15652,9 +15687,11 @@
     <col min="7" max="7" width="20.83203125" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="11" max="11" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -15673,7 +15710,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="2" spans="1:9" s="30" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:11" s="30" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="31" t="s">
@@ -15697,8 +15734,14 @@
       <c r="I2" s="31" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J2" s="88" t="s">
+        <v>303</v>
+      </c>
+      <c r="K2" s="88" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -15726,8 +15769,14 @@
       <c r="I3" s="8" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J3" s="89" t="s">
+        <v>305</v>
+      </c>
+      <c r="K3" s="89" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -15747,8 +15796,11 @@
       <c r="I4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="J4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -15769,7 +15821,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -15792,7 +15844,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -15815,7 +15867,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -15838,7 +15890,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -15861,7 +15913,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -15884,7 +15936,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -20496,7 +20548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CCD-3152 - Add event enabling condition and callback url
</commit_message>
<xml_diff>
--- a/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_CNP_RDM5118.xlsx
+++ b/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/CCD_CNP_RDM5118.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11012"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafalkalita/dev/moj/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hmcts/IdeaProjects/ccd-test-definitions/src/main/resources/uk/gov/hmcts/ccd/test_definitions/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1FA6DF-7CB2-6E47-98A1-9B9005B9D734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B1840F-0267-334B-ABF0-39B346F5441D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="56960" yWindow="6040" windowWidth="29180" windowHeight="16620" tabRatio="823" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3820" yWindow="2300" windowWidth="28800" windowHeight="17500" tabRatio="823" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7354" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7357" uniqueCount="311">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -986,7 +986,18 @@
     <t>RetriesGetCaseUrl</t>
   </si>
   <si>
-    <t>${TEST_STUB_SERVICE_BASE_URL:http://ccd-test-stubs-service-aat.service.core-compute-aat.internal}/case_type/fe-functional-test/callback_get_case</t>
+    <t>${TEST_STUB_SERVICE_BASE_URL:http://ccd-test-stubs-service-aat.service.core-compute-aat.internal}/case_type/fe-functional-test/callback_get_case_gs</t>
+  </si>
+  <si>
+    <t>Future Elements not for MVP. 
+If '*' is provided, then the current state will not change and will be same as pre condition state
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>EventEnablingCondition</t>
+  </si>
+  <si>
+    <t>[INJECTED_DATA.gsData]="GS Value"</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1009,7 @@
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="43" x14ac:knownFonts="1">
+  <fonts count="44" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1283,8 +1294,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1321,8 +1339,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0432FF"/>
+        <bgColor rgb="FF0432FF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1375,6 +1399,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1407,7 +1446,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="41" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1535,6 +1574,15 @@
     </xf>
     <xf numFmtId="49" fontId="42" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="43" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="29">
@@ -1871,7 +1919,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2993,7 +3041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F122" sqref="F122"/>
     </sheetView>
   </sheetViews>
@@ -15672,8 +15720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -15982,7 +16030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M135"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="C121" sqref="C121:C135"/>
     </sheetView>
   </sheetViews>
@@ -21102,10 +21150,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21119,17 +21167,18 @@
     <col min="7" max="7" width="12.6640625" customWidth="1"/>
     <col min="8" max="8" width="45.33203125" customWidth="1"/>
     <col min="9" max="9" width="25.6640625" customWidth="1"/>
-    <col min="10" max="10" width="29.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="32" style="30" customWidth="1"/>
-    <col min="12" max="12" width="31.33203125" style="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.83203125" style="30" customWidth="1"/>
-    <col min="14" max="14" width="26.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.33203125" style="30" customWidth="1"/>
-    <col min="16" max="16" width="23.6640625" customWidth="1"/>
-    <col min="17" max="17" width="31.1640625" customWidth="1"/>
+    <col min="10" max="10" width="42.1640625" style="14" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32" style="30" customWidth="1"/>
+    <col min="13" max="13" width="31.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.83203125" style="30" customWidth="1"/>
+    <col min="15" max="15" width="26.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.33203125" style="30" customWidth="1"/>
+    <col min="17" max="17" width="23.6640625" customWidth="1"/>
+    <col min="18" max="18" width="31.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
@@ -21147,8 +21196,9 @@
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:17" ht="84" x14ac:dyDescent="0.15">
+      <c r="J1" s="28"/>
+    </row>
+    <row r="2" spans="1:18" ht="84" x14ac:dyDescent="0.15">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
@@ -21172,32 +21222,35 @@
       <c r="I2" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="90" t="s">
+        <v>308</v>
+      </c>
+      <c r="K2" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="L2" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="M2" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="N2" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="O2" s="32" t="s">
         <v>89</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="P2" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="P2" s="31" t="s">
+      <c r="Q2" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="Q2" s="32" t="s">
+      <c r="R2" s="32" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -21225,32 +21278,35 @@
       <c r="I3" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="36" t="s">
+      <c r="J3" s="91" t="s">
+        <v>309</v>
+      </c>
+      <c r="K3" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="L3" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="36" t="s">
+      <c r="M3" s="36" t="s">
         <v>66</v>
       </c>
-      <c r="M3" s="36" t="s">
+      <c r="N3" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="36" t="s">
+      <c r="O3" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="O3" s="36" t="s">
+      <c r="P3" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="11">
         <v>42736</v>
       </c>
@@ -21272,14 +21328,15 @@
       <c r="I4" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P4" t="s">
+      <c r="J4" s="92"/>
+      <c r="Q4" t="s">
         <v>117</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="R4" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13">
         <v>42736</v>
       </c>
@@ -21303,20 +21360,23 @@
       <c r="I5" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="J5" s="30"/>
+      <c r="J5" s="92" t="s">
+        <v>310</v>
+      </c>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
       <c r="M5" s="30"/>
       <c r="N5" s="30"/>
       <c r="O5" s="30"/>
-      <c r="P5" s="14" t="s">
+      <c r="P5" s="30"/>
+      <c r="Q5" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q5" s="24" t="s">
+      <c r="R5" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="13">
         <v>42736</v>
       </c>
@@ -21340,20 +21400,21 @@
       <c r="I6" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="J6" s="30"/>
+      <c r="J6" s="42"/>
       <c r="K6" s="30"/>
       <c r="L6" s="30"/>
       <c r="M6" s="30"/>
       <c r="N6" s="30"/>
       <c r="O6" s="30"/>
-      <c r="P6" s="14" t="s">
+      <c r="P6" s="30"/>
+      <c r="Q6" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q6" s="24" t="s">
+      <c r="R6" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="13">
         <v>42736</v>
       </c>
@@ -21377,20 +21438,21 @@
       <c r="I7" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="J7" s="30"/>
+      <c r="J7" s="42"/>
       <c r="K7" s="30"/>
       <c r="L7" s="30"/>
       <c r="M7" s="30"/>
       <c r="N7" s="30"/>
       <c r="O7" s="30"/>
-      <c r="P7" s="14" t="s">
+      <c r="P7" s="30"/>
+      <c r="Q7" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q7" s="24" t="s">
+      <c r="R7" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="13">
         <v>42736</v>
       </c>
@@ -21414,20 +21476,21 @@
       <c r="I8" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="J8" s="30"/>
+      <c r="J8" s="42"/>
       <c r="K8" s="30"/>
       <c r="L8" s="30"/>
       <c r="M8" s="30"/>
       <c r="N8" s="30"/>
       <c r="O8" s="30"/>
-      <c r="P8" s="14" t="s">
+      <c r="P8" s="30"/>
+      <c r="Q8" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q8" s="24" t="s">
+      <c r="R8" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="13">
         <v>42736</v>
       </c>
@@ -21451,20 +21514,21 @@
       <c r="I9" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="J9" s="30"/>
+      <c r="J9" s="42"/>
       <c r="K9" s="30"/>
       <c r="L9" s="30"/>
       <c r="M9" s="30"/>
       <c r="N9" s="30"/>
       <c r="O9" s="30"/>
-      <c r="P9" s="14" t="s">
+      <c r="P9" s="30"/>
+      <c r="Q9" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q9" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R9" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" s="14" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13">
         <v>42736</v>
       </c>
@@ -21486,20 +21550,21 @@
       <c r="I10" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="J10" s="30"/>
+      <c r="J10" s="42"/>
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
       <c r="M10" s="30"/>
       <c r="N10" s="30"/>
       <c r="O10" s="30"/>
-      <c r="P10" s="14" t="s">
+      <c r="P10" s="30"/>
+      <c r="Q10" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q10" s="24" t="s">
+      <c r="R10" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13">
         <v>42736</v>
       </c>
@@ -21523,20 +21588,21 @@
       <c r="I11" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="J11" s="30"/>
+      <c r="J11" s="42"/>
       <c r="K11" s="30"/>
       <c r="L11" s="30"/>
       <c r="M11" s="30"/>
       <c r="N11" s="30"/>
       <c r="O11" s="30"/>
-      <c r="P11" s="14" t="s">
+      <c r="P11" s="30"/>
+      <c r="Q11" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q11" s="24" t="s">
+      <c r="R11" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13">
         <v>42736</v>
       </c>
@@ -21560,20 +21626,21 @@
       <c r="I12" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="J12" s="30"/>
+      <c r="J12" s="42"/>
       <c r="K12" s="30"/>
       <c r="L12" s="30"/>
       <c r="M12" s="30"/>
       <c r="N12" s="30"/>
       <c r="O12" s="30"/>
-      <c r="P12" s="14" t="s">
+      <c r="P12" s="30"/>
+      <c r="Q12" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q12" s="24" t="s">
+      <c r="R12" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13">
         <v>42736</v>
       </c>
@@ -21597,20 +21664,21 @@
       <c r="I13" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="J13" s="30"/>
+      <c r="J13" s="42"/>
       <c r="K13" s="30"/>
       <c r="L13" s="30"/>
       <c r="M13" s="30"/>
       <c r="N13" s="30"/>
       <c r="O13" s="30"/>
-      <c r="P13" s="14" t="s">
+      <c r="P13" s="30"/>
+      <c r="Q13" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q13" s="24" t="s">
+      <c r="R13" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13">
         <v>42736</v>
       </c>
@@ -21634,20 +21702,21 @@
       <c r="I14" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="J14" s="30"/>
+      <c r="J14" s="42"/>
       <c r="K14" s="30"/>
       <c r="L14" s="30"/>
       <c r="M14" s="30"/>
       <c r="N14" s="30"/>
       <c r="O14" s="30"/>
-      <c r="P14" s="14" t="s">
+      <c r="P14" s="30"/>
+      <c r="Q14" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q14" s="24" t="s">
+      <c r="R14" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:18" s="14" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13">
         <v>42736</v>
       </c>
@@ -21671,20 +21740,21 @@
       <c r="I15" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="J15" s="30"/>
+      <c r="J15" s="42"/>
       <c r="K15" s="30"/>
       <c r="L15" s="30"/>
       <c r="M15" s="30"/>
       <c r="N15" s="30"/>
       <c r="O15" s="30"/>
-      <c r="P15" s="14" t="s">
+      <c r="P15" s="30"/>
+      <c r="Q15" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q15" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R15" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="13">
         <v>42736</v>
       </c>
@@ -21706,14 +21776,15 @@
       <c r="I16" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P16" s="14" t="s">
+      <c r="J16" s="42"/>
+      <c r="Q16" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q16" s="24" t="s">
+      <c r="R16" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="13">
         <v>42736</v>
       </c>
@@ -21737,14 +21808,15 @@
       <c r="I17" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="P17" s="14" t="s">
+      <c r="J17" s="42"/>
+      <c r="Q17" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q17" s="24" t="s">
+      <c r="R17" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="13">
         <v>42736</v>
       </c>
@@ -21768,14 +21840,15 @@
       <c r="I18" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P18" s="14" t="s">
+      <c r="J18" s="42"/>
+      <c r="Q18" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q18" s="24" t="s">
+      <c r="R18" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="13">
         <v>42736</v>
       </c>
@@ -21799,14 +21872,15 @@
       <c r="I19" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="P19" s="14" t="s">
+      <c r="J19" s="42"/>
+      <c r="Q19" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q19" s="24" t="s">
+      <c r="R19" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="13">
         <v>42736</v>
       </c>
@@ -21830,14 +21904,15 @@
       <c r="I20" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P20" s="14" t="s">
+      <c r="J20" s="42"/>
+      <c r="Q20" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q20" s="24" t="s">
+      <c r="R20" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="13">
         <v>42736</v>
       </c>
@@ -21861,14 +21936,15 @@
       <c r="I21" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P21" s="14" t="s">
+      <c r="J21" s="42"/>
+      <c r="Q21" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q21" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R21" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="13">
         <v>42736</v>
       </c>
@@ -21890,14 +21966,15 @@
       <c r="I22" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P22" s="14" t="s">
+      <c r="J22" s="42"/>
+      <c r="Q22" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q22" s="24" t="s">
+      <c r="R22" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="13">
         <v>42736</v>
       </c>
@@ -21921,14 +21998,15 @@
       <c r="I23" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="P23" s="14" t="s">
+      <c r="J23" s="42"/>
+      <c r="Q23" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q23" s="24" t="s">
+      <c r="R23" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="13">
         <v>42736</v>
       </c>
@@ -21952,14 +22030,15 @@
       <c r="I24" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P24" s="14" t="s">
+      <c r="J24" s="42"/>
+      <c r="Q24" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q24" s="24" t="s">
+      <c r="R24" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="13">
         <v>42736</v>
       </c>
@@ -21983,14 +22062,15 @@
       <c r="I25" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="P25" s="14" t="s">
+      <c r="J25" s="42"/>
+      <c r="Q25" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q25" s="24" t="s">
+      <c r="R25" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="13">
         <v>42736</v>
       </c>
@@ -22014,14 +22094,15 @@
       <c r="I26" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P26" s="14" t="s">
+      <c r="J26" s="42"/>
+      <c r="Q26" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q26" s="24" t="s">
+      <c r="R26" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="13">
         <v>42736</v>
       </c>
@@ -22045,14 +22126,15 @@
       <c r="I27" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P27" s="14" t="s">
+      <c r="J27" s="42"/>
+      <c r="Q27" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q27" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R27" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="13">
         <v>42736</v>
       </c>
@@ -22074,14 +22156,15 @@
       <c r="I28" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P28" s="14" t="s">
+      <c r="J28" s="42"/>
+      <c r="Q28" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q28" s="24" t="s">
+      <c r="R28" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="13">
         <v>42736</v>
       </c>
@@ -22105,14 +22188,15 @@
       <c r="I29" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="P29" s="14" t="s">
+      <c r="J29" s="42"/>
+      <c r="Q29" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q29" s="24" t="s">
+      <c r="R29" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="13">
         <v>42736</v>
       </c>
@@ -22136,14 +22220,15 @@
       <c r="I30" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P30" s="14" t="s">
+      <c r="J30" s="42"/>
+      <c r="Q30" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q30" s="24" t="s">
+      <c r="R30" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="13">
         <v>42736</v>
       </c>
@@ -22167,14 +22252,15 @@
       <c r="I31" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="P31" s="14" t="s">
+      <c r="J31" s="42"/>
+      <c r="Q31" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q31" s="24" t="s">
+      <c r="R31" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="13">
         <v>42736</v>
       </c>
@@ -22198,14 +22284,15 @@
       <c r="I32" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P32" s="14" t="s">
+      <c r="J32" s="42"/>
+      <c r="Q32" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q32" s="24" t="s">
+      <c r="R32" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="13">
         <v>42736</v>
       </c>
@@ -22229,14 +22316,15 @@
       <c r="I33" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P33" s="14" t="s">
+      <c r="J33" s="42"/>
+      <c r="Q33" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q33" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R33" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="13">
         <v>42736</v>
       </c>
@@ -22258,14 +22346,15 @@
       <c r="I34" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P34" s="14" t="s">
+      <c r="J34" s="42"/>
+      <c r="Q34" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q34" s="24" t="s">
+      <c r="R34" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="13">
         <v>42736</v>
       </c>
@@ -22289,14 +22378,15 @@
       <c r="I35" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="P35" s="14" t="s">
+      <c r="J35" s="42"/>
+      <c r="Q35" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q35" s="24" t="s">
+      <c r="R35" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="13">
         <v>42736</v>
       </c>
@@ -22320,14 +22410,15 @@
       <c r="I36" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P36" s="14" t="s">
+      <c r="J36" s="42"/>
+      <c r="Q36" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q36" s="24" t="s">
+      <c r="R36" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="13">
         <v>42736</v>
       </c>
@@ -22351,14 +22442,15 @@
       <c r="I37" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="P37" s="14" t="s">
+      <c r="J37" s="42"/>
+      <c r="Q37" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q37" s="24" t="s">
+      <c r="R37" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="13">
         <v>42736</v>
       </c>
@@ -22382,14 +22474,15 @@
       <c r="I38" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P38" s="14" t="s">
+      <c r="J38" s="42"/>
+      <c r="Q38" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q38" s="24" t="s">
+      <c r="R38" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="39" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="13">
         <v>42736</v>
       </c>
@@ -22413,14 +22506,15 @@
       <c r="I39" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P39" s="14" t="s">
+      <c r="J39" s="42"/>
+      <c r="Q39" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q39" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R39" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="13">
         <v>42736</v>
       </c>
@@ -22442,14 +22536,15 @@
       <c r="I40" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P40" s="14" t="s">
+      <c r="J40" s="42"/>
+      <c r="Q40" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q40" s="24" t="s">
+      <c r="R40" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="13">
         <v>42736</v>
       </c>
@@ -22473,14 +22568,15 @@
       <c r="I41" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="P41" s="14" t="s">
+      <c r="J41" s="42"/>
+      <c r="Q41" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q41" s="24" t="s">
+      <c r="R41" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="13">
         <v>42736</v>
       </c>
@@ -22504,14 +22600,15 @@
       <c r="I42" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P42" s="14" t="s">
+      <c r="J42" s="42"/>
+      <c r="Q42" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q42" s="24" t="s">
+      <c r="R42" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="13">
         <v>42736</v>
       </c>
@@ -22535,14 +22632,15 @@
       <c r="I43" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="P43" s="14" t="s">
+      <c r="J43" s="42"/>
+      <c r="Q43" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q43" s="24" t="s">
+      <c r="R43" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="13">
         <v>42736</v>
       </c>
@@ -22566,14 +22664,15 @@
       <c r="I44" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P44" s="14" t="s">
+      <c r="J44" s="42"/>
+      <c r="Q44" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q44" s="24" t="s">
+      <c r="R44" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="13">
         <v>42736</v>
       </c>
@@ -22597,14 +22696,15 @@
       <c r="I45" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P45" s="14" t="s">
+      <c r="J45" s="42"/>
+      <c r="Q45" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q45" s="24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="R45" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="13">
         <v>42736</v>
       </c>
@@ -22626,14 +22726,15 @@
       <c r="I46" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P46" s="14" t="s">
+      <c r="J46" s="42"/>
+      <c r="Q46" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q46" s="24" t="s">
+      <c r="R46" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="13">
         <v>42736</v>
       </c>
@@ -22657,14 +22758,15 @@
       <c r="I47" s="42" t="s">
         <v>184</v>
       </c>
-      <c r="P47" s="14" t="s">
+      <c r="J47" s="42"/>
+      <c r="Q47" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q47" s="24" t="s">
+      <c r="R47" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="13">
         <v>42736</v>
       </c>
@@ -22688,14 +22790,15 @@
       <c r="I48" s="42" t="s">
         <v>183</v>
       </c>
-      <c r="P48" s="14" t="s">
+      <c r="J48" s="42"/>
+      <c r="Q48" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q48" s="24" t="s">
+      <c r="R48" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="13">
         <v>42736</v>
       </c>
@@ -22719,14 +22822,15 @@
       <c r="I49" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="P49" s="14" t="s">
+      <c r="J49" s="42"/>
+      <c r="Q49" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q49" s="24" t="s">
+      <c r="R49" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="13">
         <v>42736</v>
       </c>
@@ -22750,14 +22854,15 @@
       <c r="I50" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P50" s="14" t="s">
+      <c r="J50" s="42"/>
+      <c r="Q50" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q50" s="24" t="s">
+      <c r="R50" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="13">
         <v>42736</v>
       </c>
@@ -22781,10 +22886,11 @@
       <c r="I51" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="P51" s="14" t="s">
+      <c r="J51" s="42"/>
+      <c r="Q51" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="Q51" s="24" t="s">
+      <c r="R51" s="24" t="s">
         <v>26</v>
       </c>
     </row>
@@ -22814,7 +22920,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O355"/>
   <sheetViews>
-    <sheetView topLeftCell="A303" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C314" sqref="C314:C355"/>
     </sheetView>
   </sheetViews>

</xml_diff>